<commit_message>
Correction to option for number (removed CSBCG)
</commit_message>
<xml_diff>
--- a/app/config/tables/IDMATCH01/Forms/IDMATCH01/IDMATCH01.xlsx
+++ b/app/config/tables/IDMATCH01/Forms/IDMATCH01/IDMATCH01.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70828BF-7B21-468C-8F5A-ECA67B9ADB1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA12D39-D976-47C5-BD15-471333F06709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="728" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="349">
   <si>
     <t>setting_name</t>
   </si>
@@ -161,394 +161,922 @@
     <t>ID-01</t>
   </si>
   <si>
-    <t>SOTNUMEST203010161</t>
-  </si>
-  <si>
-    <t>images\1683463133940_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203010161</t>
-  </si>
-  <si>
-    <t>OBS203010161</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203010171</t>
-  </si>
-  <si>
-    <t>images\1676468097139_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203010171</t>
-  </si>
-  <si>
-    <t>OBS203010171</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203010191</t>
-  </si>
-  <si>
-    <t>images\1676397411271_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203010191</t>
-  </si>
-  <si>
-    <t>OBS203010191</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203010201</t>
-  </si>
-  <si>
-    <t>images\1676395922843_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203010201</t>
-  </si>
-  <si>
-    <t>OBS203010201</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203010211</t>
-  </si>
-  <si>
-    <t>images\1683466919066_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203010211</t>
-  </si>
-  <si>
-    <t>OBS203010211</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203010221</t>
-  </si>
-  <si>
-    <t>images\1697889036875_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203010221</t>
-  </si>
-  <si>
-    <t>OBS203010221</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203010261</t>
-  </si>
-  <si>
-    <t>images\1706699037866_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203010261</t>
-  </si>
-  <si>
-    <t>OBS203010261</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203010271</t>
-  </si>
-  <si>
-    <t>images\1706701136448_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203010271</t>
-  </si>
-  <si>
-    <t>OBS203010271</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203020151</t>
-  </si>
-  <si>
-    <t>images\1684835971774_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203020151</t>
-  </si>
-  <si>
-    <t>OBS203020151</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203020161</t>
-  </si>
-  <si>
-    <t>images\1677063422651_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203020161</t>
-  </si>
-  <si>
-    <t>OBS203020161</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203020281</t>
-  </si>
-  <si>
-    <t>images\1697896468920_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203020281</t>
-  </si>
-  <si>
-    <t>OBS203020281</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203020371</t>
-  </si>
-  <si>
-    <t>images\1697895396484_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203020371</t>
-  </si>
-  <si>
-    <t>OBS203020371</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203040661</t>
-  </si>
-  <si>
-    <t>images\1681913760559_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203040661</t>
-  </si>
-  <si>
-    <t>OBS203040661</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203040861</t>
-  </si>
-  <si>
-    <t>images\1691063836188_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203040861</t>
-  </si>
-  <si>
-    <t>OBS203040861</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203040981</t>
-  </si>
-  <si>
-    <t>images\1691064390025_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203040981</t>
-  </si>
-  <si>
-    <t>OBS203040981</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203041081</t>
-  </si>
-  <si>
-    <t>images\1701783222797_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203041081</t>
-  </si>
-  <si>
-    <t>OBS203041081</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203041111</t>
-  </si>
-  <si>
-    <t>images\1708261645047_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203041111</t>
-  </si>
-  <si>
-    <t>OBS203041111</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203050331</t>
-  </si>
-  <si>
-    <t>images\1670328914476_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203050331</t>
-  </si>
-  <si>
-    <t>OBS203050331</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203050341</t>
-  </si>
-  <si>
-    <t>images\1676383715974_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203050341</t>
-  </si>
-  <si>
-    <t>OBS203050341</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203050351</t>
-  </si>
-  <si>
-    <t>images\1676382550240_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203050351</t>
-  </si>
-  <si>
-    <t>OBS203050351</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203050361</t>
-  </si>
-  <si>
-    <t>images\1670329843153_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203050361</t>
-  </si>
-  <si>
-    <t>OBS203050361</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203050371</t>
-  </si>
-  <si>
-    <t>images\1679225732668_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203050371</t>
-  </si>
-  <si>
-    <t>OBS203050371</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203050391</t>
-  </si>
-  <si>
-    <t>images\1670342004296_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203050391</t>
-  </si>
-  <si>
-    <t>OBS203050391</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203050541</t>
-  </si>
-  <si>
-    <t>images\1687944493308_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203050541</t>
-  </si>
-  <si>
-    <t>OBS203050541</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203050581</t>
-  </si>
-  <si>
-    <t>images\1679227669152_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203050581</t>
-  </si>
-  <si>
-    <t>OBS203050581</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203050631</t>
-  </si>
-  <si>
-    <t>images\1710688023729_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203050631</t>
-  </si>
-  <si>
-    <t>OBS203050631</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203050641</t>
-  </si>
-  <si>
-    <t>images\1687961212073_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203050641</t>
-  </si>
-  <si>
-    <t>OBS203050641</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203050661</t>
-  </si>
-  <si>
-    <t>images\1710685995344_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203050661</t>
-  </si>
-  <si>
-    <t>OBS203050661</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203050751</t>
-  </si>
-  <si>
-    <t>images\1710671953311_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203050751</t>
-  </si>
-  <si>
-    <t>OBS203050751</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203050831</t>
-  </si>
-  <si>
-    <t>images\1710685441493_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203050831</t>
-  </si>
-  <si>
-    <t>OBS203050831</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203050861</t>
-  </si>
-  <si>
-    <t>images\1710691366285_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203050861</t>
-  </si>
-  <si>
-    <t>OBS203050861</t>
-  </si>
-  <si>
-    <t>SOTNUMEST203050881</t>
-  </si>
-  <si>
-    <t>images\1710677139866_android_id_704d8ba76e9c83e1.jpg</t>
-  </si>
-  <si>
-    <t>IMGTYPE203050881</t>
-  </si>
-  <si>
-    <t>OBS203050881</t>
-  </si>
-  <si>
     <t>display.prompt.text</t>
   </si>
   <si>
     <t>display.prompt.image</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202020141</t>
+  </si>
+  <si>
+    <t>images\1704273350920_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202020141</t>
+  </si>
+  <si>
+    <t>OBS202020141</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202030131</t>
+  </si>
+  <si>
+    <t>images\1672914276863_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202030131</t>
+  </si>
+  <si>
+    <t>OBS202030131</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202030141</t>
+  </si>
+  <si>
+    <t>images\1679397681735_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202030141</t>
+  </si>
+  <si>
+    <t>OBS202030141</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202030151</t>
+  </si>
+  <si>
+    <t>images\1687428864988_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202030151</t>
+  </si>
+  <si>
+    <t>OBS202030151</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202030161</t>
+  </si>
+  <si>
+    <t>images\1687429591002_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202030161</t>
+  </si>
+  <si>
+    <t>OBS202030161</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202030181</t>
+  </si>
+  <si>
+    <t>images\1687431901129_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202030181</t>
+  </si>
+  <si>
+    <t>OBS202030181</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202030211</t>
+  </si>
+  <si>
+    <t>images\1687433194212_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202030211</t>
+  </si>
+  <si>
+    <t>OBS202030211</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202030221</t>
+  </si>
+  <si>
+    <t>images\1679398695293_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202030221</t>
+  </si>
+  <si>
+    <t>OBS202030221</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202030231</t>
+  </si>
+  <si>
+    <t>images\1679398147275_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202030231</t>
+  </si>
+  <si>
+    <t>OBS202030231</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202030251</t>
+  </si>
+  <si>
+    <t>images\1687434056624_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202030251</t>
+  </si>
+  <si>
+    <t>OBS202030251</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202030291</t>
+  </si>
+  <si>
+    <t>images\1701938547609_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202030291</t>
+  </si>
+  <si>
+    <t>OBS202030291</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202030301</t>
+  </si>
+  <si>
+    <t>images\1701937670997_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202030301</t>
+  </si>
+  <si>
+    <t>OBS202030301</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202030311</t>
+  </si>
+  <si>
+    <t>images\1701938158086_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202030311</t>
+  </si>
+  <si>
+    <t>OBS202030311</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202030321</t>
+  </si>
+  <si>
+    <t>images\1701939925304_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202030321</t>
+  </si>
+  <si>
+    <t>OBS202030321</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202030331</t>
+  </si>
+  <si>
+    <t>images\1701941301512_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202030331</t>
+  </si>
+  <si>
+    <t>OBS202030331</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202030332</t>
+  </si>
+  <si>
+    <t>images\1701939554760_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202030332</t>
+  </si>
+  <si>
+    <t>OBS202030332</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202030341</t>
+  </si>
+  <si>
+    <t>images\1701940891700_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202030341</t>
+  </si>
+  <si>
+    <t>OBS202030341</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202040061</t>
+  </si>
+  <si>
+    <t>images\1691747287456_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202040061</t>
+  </si>
+  <si>
+    <t>OBS202040061</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202040091</t>
+  </si>
+  <si>
+    <t>images\1674643120355_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202040091</t>
+  </si>
+  <si>
+    <t>OBS202040091</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202040101</t>
+  </si>
+  <si>
+    <t>images\1691749200416_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202040101</t>
+  </si>
+  <si>
+    <t>OBS202040101</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202040111</t>
+  </si>
+  <si>
+    <t>images\1707297971652_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202040111</t>
+  </si>
+  <si>
+    <t>OBS202040111</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202040141</t>
+  </si>
+  <si>
+    <t>images\1707296670058_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202040141</t>
+  </si>
+  <si>
+    <t>OBS202040141</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202040151</t>
+  </si>
+  <si>
+    <t>images\1707294869652_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202040151</t>
+  </si>
+  <si>
+    <t>OBS202040151</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202040171</t>
+  </si>
+  <si>
+    <t>images\1707297383339_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202040171</t>
+  </si>
+  <si>
+    <t>OBS202040171</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202040181</t>
+  </si>
+  <si>
+    <t>images\1707298451846_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202040181</t>
+  </si>
+  <si>
+    <t>OBS202040181</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202050331</t>
+  </si>
+  <si>
+    <t>images\1692438314239_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202050331</t>
+  </si>
+  <si>
+    <t>OBS202050331</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202050361</t>
+  </si>
+  <si>
+    <t>images\1692433188564_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202050361</t>
+  </si>
+  <si>
+    <t>OBS202050361</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202050521</t>
+  </si>
+  <si>
+    <t>images\1709804513325_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202050521</t>
+  </si>
+  <si>
+    <t>OBS202050521</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202050551</t>
+  </si>
+  <si>
+    <t>images\1709805800581_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202050551</t>
+  </si>
+  <si>
+    <t>OBS202050551</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202060301</t>
+  </si>
+  <si>
+    <t>images\1675858575429_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202060301</t>
+  </si>
+  <si>
+    <t>OBS202060301</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202060781</t>
+  </si>
+  <si>
+    <t>images\1670850149208_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202060781</t>
+  </si>
+  <si>
+    <t>OBS202060781</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202060831</t>
+  </si>
+  <si>
+    <t>images\1670862531332_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202060831</t>
+  </si>
+  <si>
+    <t>OBS202060831</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202060851</t>
+  </si>
+  <si>
+    <t>images\1670838908799_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202060851</t>
+  </si>
+  <si>
+    <t>OBS202060851</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202060871</t>
+  </si>
+  <si>
+    <t>images\1670843327224_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202060871</t>
+  </si>
+  <si>
+    <t>OBS202060871</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202060911</t>
+  </si>
+  <si>
+    <t>images\1670849458528_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202060911</t>
+  </si>
+  <si>
+    <t>OBS202060911</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202060971</t>
+  </si>
+  <si>
+    <t>images\1682421618863_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202060971</t>
+  </si>
+  <si>
+    <t>OBS202060971</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202060991</t>
+  </si>
+  <si>
+    <t>images\1670848119425_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202060991</t>
+  </si>
+  <si>
+    <t>OBS202060991</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202061001</t>
+  </si>
+  <si>
+    <t>images\1677234896833_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202061001</t>
+  </si>
+  <si>
+    <t>OBS202061001</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202061002</t>
+  </si>
+  <si>
+    <t>images\1677234634088_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202061002</t>
+  </si>
+  <si>
+    <t>OBS202061002</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202061031</t>
+  </si>
+  <si>
+    <t>images\1675859669528_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202061031</t>
+  </si>
+  <si>
+    <t>OBS202061031</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202061041</t>
+  </si>
+  <si>
+    <t>images\1682417415526_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202061041</t>
+  </si>
+  <si>
+    <t>OBS202061041</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202061051</t>
+  </si>
+  <si>
+    <t>images\1681391627531_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202061051</t>
+  </si>
+  <si>
+    <t>OBS202061051</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202061101</t>
+  </si>
+  <si>
+    <t>images\1692784917359_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202061101</t>
+  </si>
+  <si>
+    <t>OBS202061101</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202061121</t>
+  </si>
+  <si>
+    <t>images\1692786244537_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202061121</t>
+  </si>
+  <si>
+    <t>OBS202061121</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202061211</t>
+  </si>
+  <si>
+    <t>images\1692796876943_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202061211</t>
+  </si>
+  <si>
+    <t>OBS202061211</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202061251</t>
+  </si>
+  <si>
+    <t>images\1692792473231_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202061251</t>
+  </si>
+  <si>
+    <t>OBS202061251</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202061271</t>
+  </si>
+  <si>
+    <t>images\1710153279091_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202061271</t>
+  </si>
+  <si>
+    <t>OBS202061271</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202061281</t>
+  </si>
+  <si>
+    <t>images\1700212152127_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202061281</t>
+  </si>
+  <si>
+    <t>OBS202061281</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202061301</t>
+  </si>
+  <si>
+    <t>images\1700214883268_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202061301</t>
+  </si>
+  <si>
+    <t>OBS202061301</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202090091</t>
+  </si>
+  <si>
+    <t>images\1689350341716_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202090091</t>
+  </si>
+  <si>
+    <t>OBS202090091</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202090111</t>
+  </si>
+  <si>
+    <t>images\1689352765811_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202090111</t>
+  </si>
+  <si>
+    <t>OBS202090111</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202100151</t>
+  </si>
+  <si>
+    <t>images\1674646135993_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202100151</t>
+  </si>
+  <si>
+    <t>OBS202100151</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202110181</t>
+  </si>
+  <si>
+    <t>images\1673950961798_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202110181</t>
+  </si>
+  <si>
+    <t>OBS202110181</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202110251</t>
+  </si>
+  <si>
+    <t>images\1686042786510_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202110251</t>
+  </si>
+  <si>
+    <t>OBS202110251</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202120331</t>
+  </si>
+  <si>
+    <t>images\1688987197431_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202120331</t>
+  </si>
+  <si>
+    <t>OBS202120331</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202120391</t>
+  </si>
+  <si>
+    <t>images\1688984571584_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202120391</t>
+  </si>
+  <si>
+    <t>OBS202120391</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202120451</t>
+  </si>
+  <si>
+    <t>images\1709194825776_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202120451</t>
+  </si>
+  <si>
+    <t>OBS202120451</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202120461</t>
+  </si>
+  <si>
+    <t>images\1709196651156_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202120461</t>
+  </si>
+  <si>
+    <t>OBS202120461</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202120471</t>
+  </si>
+  <si>
+    <t>images\1709196007018_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202120471</t>
+  </si>
+  <si>
+    <t>OBS202120471</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202130311</t>
+  </si>
+  <si>
+    <t>images\1673954833403_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202130311</t>
+  </si>
+  <si>
+    <t>OBS202130311</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202140181</t>
+  </si>
+  <si>
+    <t>images\1688652180354_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202140181</t>
+  </si>
+  <si>
+    <t>OBS202140181</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202140331</t>
+  </si>
+  <si>
+    <t>images\1710855691833_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202140331</t>
+  </si>
+  <si>
+    <t>OBS202140331</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202170111</t>
+  </si>
+  <si>
+    <t>images\1667897263565_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202170111</t>
+  </si>
+  <si>
+    <t>OBS202170111</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202170121</t>
+  </si>
+  <si>
+    <t>images\1690364381705_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202170121</t>
+  </si>
+  <si>
+    <t>OBS202170121</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202170131</t>
+  </si>
+  <si>
+    <t>images\1673528662997_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202170131</t>
+  </si>
+  <si>
+    <t>OBS202170131</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202170141</t>
+  </si>
+  <si>
+    <t>images\1673528240827_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202170141</t>
+  </si>
+  <si>
+    <t>OBS202170141</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202170161</t>
+  </si>
+  <si>
+    <t>images\1673529793738_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202170161</t>
+  </si>
+  <si>
+    <t>OBS202170161</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202170181</t>
+  </si>
+  <si>
+    <t>images\1690363961658_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202170181</t>
+  </si>
+  <si>
+    <t>OBS202170181</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202170191</t>
+  </si>
+  <si>
+    <t>images\1695380175173_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202170191</t>
+  </si>
+  <si>
+    <t>OBS202170191</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202170211</t>
+  </si>
+  <si>
+    <t>images\1690537841895_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202170211</t>
+  </si>
+  <si>
+    <t>OBS202170211</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202170231</t>
+  </si>
+  <si>
+    <t>images\1690367902812_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202170231</t>
+  </si>
+  <si>
+    <t>OBS202170231</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202170251</t>
+  </si>
+  <si>
+    <t>images\1690534820274_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202170251</t>
+  </si>
+  <si>
+    <t>OBS202170251</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202170261</t>
+  </si>
+  <si>
+    <t>images\1690533785428_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202170261</t>
+  </si>
+  <si>
+    <t>OBS202170261</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202170271</t>
+  </si>
+  <si>
+    <t>images\1698658806845_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202170271</t>
+  </si>
+  <si>
+    <t>OBS202170271</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202170281</t>
+  </si>
+  <si>
+    <t>images\1707293713388_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202170281</t>
+  </si>
+  <si>
+    <t>OBS202170281</t>
+  </si>
+  <si>
+    <t>SOTNUMEST202170291</t>
+  </si>
+  <si>
+    <t>images\1707210733703_android_id_6a4a34b9b66195cd.jpg</t>
+  </si>
+  <si>
+    <t>IMGTYPE202170291</t>
+  </si>
+  <si>
+    <t>OBS202170291</t>
   </si>
 </sst>
 </file>
@@ -1034,11 +1562,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
-  <dimension ref="A1:F161"/>
+  <dimension ref="A1:F381"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1065,10 +1593,10 @@
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>171</v>
+        <v>43</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>172</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1081,13 +1609,13 @@
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
         <v>33</v>
       </c>
       <c r="F3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -1098,7 +1626,7 @@
         <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
@@ -1109,7 +1637,7 @@
         <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -1126,17 +1654,18 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="4"/>
       <c r="B8" t="s">
         <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E8" t="s">
         <v>33</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -1147,7 +1676,7 @@
         <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E9" t="s">
         <v>34</v>
@@ -1158,14 +1687,14 @@
         <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E10" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
+      <c r="A11" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1179,13 +1708,13 @@
         <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E13" t="s">
         <v>33</v>
       </c>
       <c r="F13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -1196,7 +1725,7 @@
         <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E14" t="s">
         <v>34</v>
@@ -1207,7 +1736,7 @@
         <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E15" t="s">
         <v>25</v>
@@ -1228,13 +1757,13 @@
         <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E18" t="s">
         <v>33</v>
       </c>
       <c r="F18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -1245,7 +1774,7 @@
         <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E19" t="s">
         <v>34</v>
@@ -1256,7 +1785,7 @@
         <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E20" t="s">
         <v>25</v>
@@ -1277,13 +1806,13 @@
         <v>23</v>
       </c>
       <c r="D23" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E23" t="s">
         <v>33</v>
       </c>
       <c r="F23" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
@@ -1294,7 +1823,7 @@
         <v>26</v>
       </c>
       <c r="D24" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E24" t="s">
         <v>34</v>
@@ -1305,7 +1834,7 @@
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E25" t="s">
         <v>25</v>
@@ -1326,13 +1855,13 @@
         <v>23</v>
       </c>
       <c r="D28" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E28" t="s">
         <v>33</v>
       </c>
       <c r="F28" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
@@ -1343,7 +1872,7 @@
         <v>26</v>
       </c>
       <c r="D29" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E29" t="s">
         <v>34</v>
@@ -1354,7 +1883,7 @@
         <v>24</v>
       </c>
       <c r="D30" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E30" t="s">
         <v>25</v>
@@ -1375,13 +1904,13 @@
         <v>23</v>
       </c>
       <c r="D33" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E33" t="s">
         <v>33</v>
       </c>
       <c r="F33" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
@@ -1392,7 +1921,7 @@
         <v>26</v>
       </c>
       <c r="D34" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E34" t="s">
         <v>34</v>
@@ -1403,7 +1932,7 @@
         <v>24</v>
       </c>
       <c r="D35" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E35" t="s">
         <v>25</v>
@@ -1424,13 +1953,13 @@
         <v>23</v>
       </c>
       <c r="D38" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E38" t="s">
         <v>33</v>
       </c>
       <c r="F38" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
@@ -1441,7 +1970,7 @@
         <v>26</v>
       </c>
       <c r="D39" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E39" t="s">
         <v>34</v>
@@ -1452,7 +1981,7 @@
         <v>24</v>
       </c>
       <c r="D40" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E40" t="s">
         <v>25</v>
@@ -1473,13 +2002,13 @@
         <v>23</v>
       </c>
       <c r="D43" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E43" t="s">
         <v>33</v>
       </c>
       <c r="F43" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
@@ -1490,7 +2019,7 @@
         <v>26</v>
       </c>
       <c r="D44" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E44" t="s">
         <v>34</v>
@@ -1501,7 +2030,7 @@
         <v>24</v>
       </c>
       <c r="D45" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E45" t="s">
         <v>25</v>
@@ -1522,13 +2051,13 @@
         <v>23</v>
       </c>
       <c r="D48" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E48" t="s">
         <v>33</v>
       </c>
       <c r="F48" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
@@ -1539,7 +2068,7 @@
         <v>26</v>
       </c>
       <c r="D49" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E49" t="s">
         <v>34</v>
@@ -1550,7 +2079,7 @@
         <v>24</v>
       </c>
       <c r="D50" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E50" t="s">
         <v>25</v>
@@ -1571,13 +2100,13 @@
         <v>23</v>
       </c>
       <c r="D53" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E53" t="s">
         <v>33</v>
       </c>
       <c r="F53" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
@@ -1588,7 +2117,7 @@
         <v>26</v>
       </c>
       <c r="D54" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E54" t="s">
         <v>34</v>
@@ -1599,7 +2128,7 @@
         <v>24</v>
       </c>
       <c r="D55" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E55" t="s">
         <v>25</v>
@@ -1620,13 +2149,13 @@
         <v>23</v>
       </c>
       <c r="D58" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E58" t="s">
         <v>33</v>
       </c>
       <c r="F58" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
@@ -1637,7 +2166,7 @@
         <v>26</v>
       </c>
       <c r="D59" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E59" t="s">
         <v>34</v>
@@ -1648,7 +2177,7 @@
         <v>24</v>
       </c>
       <c r="D60" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E60" t="s">
         <v>25</v>
@@ -1669,13 +2198,13 @@
         <v>23</v>
       </c>
       <c r="D63" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E63" t="s">
         <v>33</v>
       </c>
       <c r="F63" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
@@ -1686,7 +2215,7 @@
         <v>26</v>
       </c>
       <c r="D64" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E64" t="s">
         <v>34</v>
@@ -1697,7 +2226,7 @@
         <v>24</v>
       </c>
       <c r="D65" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E65" t="s">
         <v>25</v>
@@ -1718,13 +2247,13 @@
         <v>23</v>
       </c>
       <c r="D68" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E68" t="s">
         <v>33</v>
       </c>
       <c r="F68" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
@@ -1735,7 +2264,7 @@
         <v>26</v>
       </c>
       <c r="D69" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E69" t="s">
         <v>34</v>
@@ -1746,7 +2275,7 @@
         <v>24</v>
       </c>
       <c r="D70" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E70" t="s">
         <v>25</v>
@@ -1767,13 +2296,13 @@
         <v>23</v>
       </c>
       <c r="D73" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E73" t="s">
         <v>33</v>
       </c>
       <c r="F73" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
@@ -1784,7 +2313,7 @@
         <v>26</v>
       </c>
       <c r="D74" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E74" t="s">
         <v>34</v>
@@ -1795,7 +2324,7 @@
         <v>24</v>
       </c>
       <c r="D75" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E75" t="s">
         <v>25</v>
@@ -1816,13 +2345,13 @@
         <v>23</v>
       </c>
       <c r="D78" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E78" t="s">
         <v>33</v>
       </c>
       <c r="F78" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.35">
@@ -1833,7 +2362,7 @@
         <v>26</v>
       </c>
       <c r="D79" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E79" t="s">
         <v>34</v>
@@ -1844,7 +2373,7 @@
         <v>24</v>
       </c>
       <c r="D80" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E80" t="s">
         <v>25</v>
@@ -1865,13 +2394,13 @@
         <v>23</v>
       </c>
       <c r="D83" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E83" t="s">
         <v>33</v>
       </c>
       <c r="F83" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.35">
@@ -1882,7 +2411,7 @@
         <v>26</v>
       </c>
       <c r="D84" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E84" t="s">
         <v>34</v>
@@ -1893,7 +2422,7 @@
         <v>24</v>
       </c>
       <c r="D85" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E85" t="s">
         <v>25</v>
@@ -1914,13 +2443,13 @@
         <v>23</v>
       </c>
       <c r="D88" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E88" t="s">
         <v>33</v>
       </c>
       <c r="F88" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.35">
@@ -1931,7 +2460,7 @@
         <v>26</v>
       </c>
       <c r="D89" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E89" t="s">
         <v>34</v>
@@ -1942,7 +2471,7 @@
         <v>24</v>
       </c>
       <c r="D90" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E90" t="s">
         <v>25</v>
@@ -1963,13 +2492,13 @@
         <v>23</v>
       </c>
       <c r="D93" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E93" t="s">
         <v>33</v>
       </c>
       <c r="F93" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.35">
@@ -1980,7 +2509,7 @@
         <v>26</v>
       </c>
       <c r="D94" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E94" t="s">
         <v>34</v>
@@ -1991,7 +2520,7 @@
         <v>24</v>
       </c>
       <c r="D95" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E95" t="s">
         <v>25</v>
@@ -2012,13 +2541,13 @@
         <v>23</v>
       </c>
       <c r="D98" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E98" t="s">
         <v>33</v>
       </c>
       <c r="F98" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.35">
@@ -2029,7 +2558,7 @@
         <v>26</v>
       </c>
       <c r="D99" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E99" t="s">
         <v>34</v>
@@ -2040,7 +2569,7 @@
         <v>24</v>
       </c>
       <c r="D100" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E100" t="s">
         <v>25</v>
@@ -2061,13 +2590,13 @@
         <v>23</v>
       </c>
       <c r="D103" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E103" t="s">
         <v>33</v>
       </c>
       <c r="F103" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.35">
@@ -2078,7 +2607,7 @@
         <v>26</v>
       </c>
       <c r="D104" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E104" t="s">
         <v>34</v>
@@ -2089,7 +2618,7 @@
         <v>24</v>
       </c>
       <c r="D105" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E105" t="s">
         <v>25</v>
@@ -2110,13 +2639,13 @@
         <v>23</v>
       </c>
       <c r="D108" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E108" t="s">
         <v>33</v>
       </c>
       <c r="F108" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.35">
@@ -2127,7 +2656,7 @@
         <v>26</v>
       </c>
       <c r="D109" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E109" t="s">
         <v>34</v>
@@ -2138,7 +2667,7 @@
         <v>24</v>
       </c>
       <c r="D110" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E110" t="s">
         <v>25</v>
@@ -2159,13 +2688,13 @@
         <v>23</v>
       </c>
       <c r="D113" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E113" t="s">
         <v>33</v>
       </c>
       <c r="F113" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.35">
@@ -2176,7 +2705,7 @@
         <v>26</v>
       </c>
       <c r="D114" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E114" t="s">
         <v>34</v>
@@ -2187,7 +2716,7 @@
         <v>24</v>
       </c>
       <c r="D115" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E115" t="s">
         <v>25</v>
@@ -2208,13 +2737,13 @@
         <v>23</v>
       </c>
       <c r="D118" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E118" t="s">
         <v>33</v>
       </c>
       <c r="F118" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.35">
@@ -2225,7 +2754,7 @@
         <v>26</v>
       </c>
       <c r="D119" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E119" t="s">
         <v>34</v>
@@ -2236,7 +2765,7 @@
         <v>24</v>
       </c>
       <c r="D120" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E120" t="s">
         <v>25</v>
@@ -2257,13 +2786,13 @@
         <v>23</v>
       </c>
       <c r="D123" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E123" t="s">
         <v>33</v>
       </c>
       <c r="F123" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.35">
@@ -2274,7 +2803,7 @@
         <v>26</v>
       </c>
       <c r="D124" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E124" t="s">
         <v>34</v>
@@ -2285,7 +2814,7 @@
         <v>24</v>
       </c>
       <c r="D125" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E125" t="s">
         <v>25</v>
@@ -2306,13 +2835,13 @@
         <v>23</v>
       </c>
       <c r="D128" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E128" t="s">
         <v>33</v>
       </c>
       <c r="F128" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.35">
@@ -2323,7 +2852,7 @@
         <v>26</v>
       </c>
       <c r="D129" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E129" t="s">
         <v>34</v>
@@ -2334,7 +2863,7 @@
         <v>24</v>
       </c>
       <c r="D130" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E130" t="s">
         <v>25</v>
@@ -2355,13 +2884,13 @@
         <v>23</v>
       </c>
       <c r="D133" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E133" t="s">
         <v>33</v>
       </c>
       <c r="F133" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.35">
@@ -2372,7 +2901,7 @@
         <v>26</v>
       </c>
       <c r="D134" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E134" t="s">
         <v>34</v>
@@ -2383,7 +2912,7 @@
         <v>24</v>
       </c>
       <c r="D135" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E135" t="s">
         <v>25</v>
@@ -2404,13 +2933,13 @@
         <v>23</v>
       </c>
       <c r="D138" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E138" t="s">
         <v>33</v>
       </c>
       <c r="F138" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.35">
@@ -2421,7 +2950,7 @@
         <v>26</v>
       </c>
       <c r="D139" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E139" t="s">
         <v>34</v>
@@ -2432,7 +2961,7 @@
         <v>24</v>
       </c>
       <c r="D140" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E140" t="s">
         <v>25</v>
@@ -2453,13 +2982,13 @@
         <v>23</v>
       </c>
       <c r="D143" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E143" t="s">
         <v>33</v>
       </c>
       <c r="F143" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.35">
@@ -2470,7 +2999,7 @@
         <v>26</v>
       </c>
       <c r="D144" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E144" t="s">
         <v>34</v>
@@ -2481,7 +3010,7 @@
         <v>24</v>
       </c>
       <c r="D145" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E145" t="s">
         <v>25</v>
@@ -2502,13 +3031,13 @@
         <v>23</v>
       </c>
       <c r="D148" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E148" t="s">
         <v>33</v>
       </c>
       <c r="F148" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.35">
@@ -2519,7 +3048,7 @@
         <v>26</v>
       </c>
       <c r="D149" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E149" t="s">
         <v>34</v>
@@ -2530,7 +3059,7 @@
         <v>24</v>
       </c>
       <c r="D150" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E150" t="s">
         <v>25</v>
@@ -2551,13 +3080,13 @@
         <v>23</v>
       </c>
       <c r="D153" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E153" t="s">
         <v>33</v>
       </c>
       <c r="F153" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.35">
@@ -2568,7 +3097,7 @@
         <v>26</v>
       </c>
       <c r="D154" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E154" t="s">
         <v>34</v>
@@ -2579,7 +3108,7 @@
         <v>24</v>
       </c>
       <c r="D155" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E155" t="s">
         <v>25</v>
@@ -2600,13 +3129,13 @@
         <v>23</v>
       </c>
       <c r="D158" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E158" t="s">
         <v>33</v>
       </c>
       <c r="F158" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.35">
@@ -2617,7 +3146,7 @@
         <v>26</v>
       </c>
       <c r="D159" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E159" t="s">
         <v>34</v>
@@ -2628,14 +3157,2170 @@
         <v>24</v>
       </c>
       <c r="D160" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E160" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B163" t="s">
+        <v>23</v>
+      </c>
+      <c r="D163" t="s">
+        <v>173</v>
+      </c>
+      <c r="E163" t="s">
+        <v>33</v>
+      </c>
+      <c r="F163" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B164" t="s">
+        <v>32</v>
+      </c>
+      <c r="C164" t="s">
+        <v>26</v>
+      </c>
+      <c r="D164" t="s">
+        <v>175</v>
+      </c>
+      <c r="E164" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B165" t="s">
+        <v>24</v>
+      </c>
+      <c r="D165" t="s">
+        <v>176</v>
+      </c>
+      <c r="E165" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A166" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A167" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B168" t="s">
+        <v>23</v>
+      </c>
+      <c r="D168" t="s">
+        <v>177</v>
+      </c>
+      <c r="E168" t="s">
+        <v>33</v>
+      </c>
+      <c r="F168" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B169" t="s">
+        <v>32</v>
+      </c>
+      <c r="C169" t="s">
+        <v>26</v>
+      </c>
+      <c r="D169" t="s">
+        <v>179</v>
+      </c>
+      <c r="E169" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B170" t="s">
+        <v>24</v>
+      </c>
+      <c r="D170" t="s">
+        <v>180</v>
+      </c>
+      <c r="E170" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A172" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B173" t="s">
+        <v>23</v>
+      </c>
+      <c r="D173" t="s">
+        <v>181</v>
+      </c>
+      <c r="E173" t="s">
+        <v>33</v>
+      </c>
+      <c r="F173" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B174" t="s">
+        <v>32</v>
+      </c>
+      <c r="C174" t="s">
+        <v>26</v>
+      </c>
+      <c r="D174" t="s">
+        <v>183</v>
+      </c>
+      <c r="E174" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B175" t="s">
+        <v>24</v>
+      </c>
+      <c r="D175" t="s">
+        <v>184</v>
+      </c>
+      <c r="E175" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A176" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A177" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B178" t="s">
+        <v>23</v>
+      </c>
+      <c r="D178" t="s">
+        <v>185</v>
+      </c>
+      <c r="E178" t="s">
+        <v>33</v>
+      </c>
+      <c r="F178" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B179" t="s">
+        <v>32</v>
+      </c>
+      <c r="C179" t="s">
+        <v>26</v>
+      </c>
+      <c r="D179" t="s">
+        <v>187</v>
+      </c>
+      <c r="E179" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B180" t="s">
+        <v>24</v>
+      </c>
+      <c r="D180" t="s">
+        <v>188</v>
+      </c>
+      <c r="E180" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A181" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A182" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B183" t="s">
+        <v>23</v>
+      </c>
+      <c r="D183" t="s">
+        <v>189</v>
+      </c>
+      <c r="E183" t="s">
+        <v>33</v>
+      </c>
+      <c r="F183" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B184" t="s">
+        <v>32</v>
+      </c>
+      <c r="C184" t="s">
+        <v>26</v>
+      </c>
+      <c r="D184" t="s">
+        <v>191</v>
+      </c>
+      <c r="E184" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B185" t="s">
+        <v>24</v>
+      </c>
+      <c r="D185" t="s">
+        <v>192</v>
+      </c>
+      <c r="E185" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A186" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A187" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B188" t="s">
+        <v>23</v>
+      </c>
+      <c r="D188" t="s">
+        <v>193</v>
+      </c>
+      <c r="E188" t="s">
+        <v>33</v>
+      </c>
+      <c r="F188" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B189" t="s">
+        <v>32</v>
+      </c>
+      <c r="C189" t="s">
+        <v>26</v>
+      </c>
+      <c r="D189" t="s">
+        <v>195</v>
+      </c>
+      <c r="E189" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B190" t="s">
+        <v>24</v>
+      </c>
+      <c r="D190" t="s">
+        <v>196</v>
+      </c>
+      <c r="E190" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A191" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A192" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B193" t="s">
+        <v>23</v>
+      </c>
+      <c r="D193" t="s">
+        <v>197</v>
+      </c>
+      <c r="E193" t="s">
+        <v>33</v>
+      </c>
+      <c r="F193" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B194" t="s">
+        <v>32</v>
+      </c>
+      <c r="C194" t="s">
+        <v>26</v>
+      </c>
+      <c r="D194" t="s">
+        <v>199</v>
+      </c>
+      <c r="E194" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B195" t="s">
+        <v>24</v>
+      </c>
+      <c r="D195" t="s">
+        <v>200</v>
+      </c>
+      <c r="E195" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A196" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A197" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B198" t="s">
+        <v>23</v>
+      </c>
+      <c r="D198" t="s">
+        <v>201</v>
+      </c>
+      <c r="E198" t="s">
+        <v>33</v>
+      </c>
+      <c r="F198" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B199" t="s">
+        <v>32</v>
+      </c>
+      <c r="C199" t="s">
+        <v>26</v>
+      </c>
+      <c r="D199" t="s">
+        <v>203</v>
+      </c>
+      <c r="E199" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B200" t="s">
+        <v>24</v>
+      </c>
+      <c r="D200" t="s">
+        <v>204</v>
+      </c>
+      <c r="E200" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A201" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A202" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B203" t="s">
+        <v>23</v>
+      </c>
+      <c r="D203" t="s">
+        <v>205</v>
+      </c>
+      <c r="E203" t="s">
+        <v>33</v>
+      </c>
+      <c r="F203" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B204" t="s">
+        <v>32</v>
+      </c>
+      <c r="C204" t="s">
+        <v>26</v>
+      </c>
+      <c r="D204" t="s">
+        <v>207</v>
+      </c>
+      <c r="E204" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B205" t="s">
+        <v>24</v>
+      </c>
+      <c r="D205" t="s">
+        <v>208</v>
+      </c>
+      <c r="E205" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A206" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A207" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B208" t="s">
+        <v>23</v>
+      </c>
+      <c r="D208" t="s">
+        <v>209</v>
+      </c>
+      <c r="E208" t="s">
+        <v>33</v>
+      </c>
+      <c r="F208" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B209" t="s">
+        <v>32</v>
+      </c>
+      <c r="C209" t="s">
+        <v>26</v>
+      </c>
+      <c r="D209" t="s">
+        <v>211</v>
+      </c>
+      <c r="E209" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B210" t="s">
+        <v>24</v>
+      </c>
+      <c r="D210" t="s">
+        <v>212</v>
+      </c>
+      <c r="E210" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A211" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A212" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B213" t="s">
+        <v>23</v>
+      </c>
+      <c r="D213" t="s">
+        <v>213</v>
+      </c>
+      <c r="E213" t="s">
+        <v>33</v>
+      </c>
+      <c r="F213" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B214" t="s">
+        <v>32</v>
+      </c>
+      <c r="C214" t="s">
+        <v>26</v>
+      </c>
+      <c r="D214" t="s">
+        <v>215</v>
+      </c>
+      <c r="E214" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B215" t="s">
+        <v>24</v>
+      </c>
+      <c r="D215" t="s">
+        <v>216</v>
+      </c>
+      <c r="E215" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A216" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A217" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B218" t="s">
+        <v>23</v>
+      </c>
+      <c r="D218" t="s">
+        <v>217</v>
+      </c>
+      <c r="E218" t="s">
+        <v>33</v>
+      </c>
+      <c r="F218" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B219" t="s">
+        <v>32</v>
+      </c>
+      <c r="C219" t="s">
+        <v>26</v>
+      </c>
+      <c r="D219" t="s">
+        <v>219</v>
+      </c>
+      <c r="E219" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B220" t="s">
+        <v>24</v>
+      </c>
+      <c r="D220" t="s">
+        <v>220</v>
+      </c>
+      <c r="E220" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A221" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A222" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B223" t="s">
+        <v>23</v>
+      </c>
+      <c r="D223" t="s">
+        <v>221</v>
+      </c>
+      <c r="E223" t="s">
+        <v>33</v>
+      </c>
+      <c r="F223" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B224" t="s">
+        <v>32</v>
+      </c>
+      <c r="C224" t="s">
+        <v>26</v>
+      </c>
+      <c r="D224" t="s">
+        <v>223</v>
+      </c>
+      <c r="E224" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B225" t="s">
+        <v>24</v>
+      </c>
+      <c r="D225" t="s">
+        <v>224</v>
+      </c>
+      <c r="E225" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A226" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A227" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B228" t="s">
+        <v>23</v>
+      </c>
+      <c r="D228" t="s">
+        <v>225</v>
+      </c>
+      <c r="E228" t="s">
+        <v>33</v>
+      </c>
+      <c r="F228" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B229" t="s">
+        <v>32</v>
+      </c>
+      <c r="C229" t="s">
+        <v>26</v>
+      </c>
+      <c r="D229" t="s">
+        <v>227</v>
+      </c>
+      <c r="E229" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B230" t="s">
+        <v>24</v>
+      </c>
+      <c r="D230" t="s">
+        <v>228</v>
+      </c>
+      <c r="E230" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A231" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A232" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B233" t="s">
+        <v>23</v>
+      </c>
+      <c r="D233" t="s">
+        <v>229</v>
+      </c>
+      <c r="E233" t="s">
+        <v>33</v>
+      </c>
+      <c r="F233" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B234" t="s">
+        <v>32</v>
+      </c>
+      <c r="C234" t="s">
+        <v>26</v>
+      </c>
+      <c r="D234" t="s">
+        <v>231</v>
+      </c>
+      <c r="E234" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B235" t="s">
+        <v>24</v>
+      </c>
+      <c r="D235" t="s">
+        <v>232</v>
+      </c>
+      <c r="E235" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A236" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A237" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B238" t="s">
+        <v>23</v>
+      </c>
+      <c r="D238" t="s">
+        <v>233</v>
+      </c>
+      <c r="E238" t="s">
+        <v>33</v>
+      </c>
+      <c r="F238" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B239" t="s">
+        <v>32</v>
+      </c>
+      <c r="C239" t="s">
+        <v>26</v>
+      </c>
+      <c r="D239" t="s">
+        <v>235</v>
+      </c>
+      <c r="E239" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B240" t="s">
+        <v>24</v>
+      </c>
+      <c r="D240" t="s">
+        <v>236</v>
+      </c>
+      <c r="E240" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A241" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A242" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B243" t="s">
+        <v>23</v>
+      </c>
+      <c r="D243" t="s">
+        <v>237</v>
+      </c>
+      <c r="E243" t="s">
+        <v>33</v>
+      </c>
+      <c r="F243" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B244" t="s">
+        <v>32</v>
+      </c>
+      <c r="C244" t="s">
+        <v>26</v>
+      </c>
+      <c r="D244" t="s">
+        <v>239</v>
+      </c>
+      <c r="E244" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B245" t="s">
+        <v>24</v>
+      </c>
+      <c r="D245" t="s">
+        <v>240</v>
+      </c>
+      <c r="E245" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A246" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A247" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B248" t="s">
+        <v>23</v>
+      </c>
+      <c r="D248" t="s">
+        <v>241</v>
+      </c>
+      <c r="E248" t="s">
+        <v>33</v>
+      </c>
+      <c r="F248" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B249" t="s">
+        <v>32</v>
+      </c>
+      <c r="C249" t="s">
+        <v>26</v>
+      </c>
+      <c r="D249" t="s">
+        <v>243</v>
+      </c>
+      <c r="E249" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B250" t="s">
+        <v>24</v>
+      </c>
+      <c r="D250" t="s">
+        <v>244</v>
+      </c>
+      <c r="E250" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A251" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A252" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B253" t="s">
+        <v>23</v>
+      </c>
+      <c r="D253" t="s">
+        <v>245</v>
+      </c>
+      <c r="E253" t="s">
+        <v>33</v>
+      </c>
+      <c r="F253" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B254" t="s">
+        <v>32</v>
+      </c>
+      <c r="C254" t="s">
+        <v>26</v>
+      </c>
+      <c r="D254" t="s">
+        <v>247</v>
+      </c>
+      <c r="E254" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B255" t="s">
+        <v>24</v>
+      </c>
+      <c r="D255" t="s">
+        <v>248</v>
+      </c>
+      <c r="E255" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A256" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A257" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B258" t="s">
+        <v>23</v>
+      </c>
+      <c r="D258" t="s">
+        <v>249</v>
+      </c>
+      <c r="E258" t="s">
+        <v>33</v>
+      </c>
+      <c r="F258" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B259" t="s">
+        <v>32</v>
+      </c>
+      <c r="C259" t="s">
+        <v>26</v>
+      </c>
+      <c r="D259" t="s">
+        <v>251</v>
+      </c>
+      <c r="E259" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B260" t="s">
+        <v>24</v>
+      </c>
+      <c r="D260" t="s">
+        <v>252</v>
+      </c>
+      <c r="E260" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A261" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A262" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B263" t="s">
+        <v>23</v>
+      </c>
+      <c r="D263" t="s">
+        <v>253</v>
+      </c>
+      <c r="E263" t="s">
+        <v>33</v>
+      </c>
+      <c r="F263" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B264" t="s">
+        <v>32</v>
+      </c>
+      <c r="C264" t="s">
+        <v>26</v>
+      </c>
+      <c r="D264" t="s">
+        <v>255</v>
+      </c>
+      <c r="E264" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B265" t="s">
+        <v>24</v>
+      </c>
+      <c r="D265" t="s">
+        <v>256</v>
+      </c>
+      <c r="E265" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A266" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A267" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B268" t="s">
+        <v>23</v>
+      </c>
+      <c r="D268" t="s">
+        <v>257</v>
+      </c>
+      <c r="E268" t="s">
+        <v>33</v>
+      </c>
+      <c r="F268" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B269" t="s">
+        <v>32</v>
+      </c>
+      <c r="C269" t="s">
+        <v>26</v>
+      </c>
+      <c r="D269" t="s">
+        <v>259</v>
+      </c>
+      <c r="E269" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B270" t="s">
+        <v>24</v>
+      </c>
+      <c r="D270" t="s">
+        <v>260</v>
+      </c>
+      <c r="E270" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A271" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A272" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B273" t="s">
+        <v>23</v>
+      </c>
+      <c r="D273" t="s">
+        <v>261</v>
+      </c>
+      <c r="E273" t="s">
+        <v>33</v>
+      </c>
+      <c r="F273" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B274" t="s">
+        <v>32</v>
+      </c>
+      <c r="C274" t="s">
+        <v>26</v>
+      </c>
+      <c r="D274" t="s">
+        <v>263</v>
+      </c>
+      <c r="E274" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B275" t="s">
+        <v>24</v>
+      </c>
+      <c r="D275" t="s">
+        <v>264</v>
+      </c>
+      <c r="E275" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A276" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A277" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B278" t="s">
+        <v>23</v>
+      </c>
+      <c r="D278" t="s">
+        <v>265</v>
+      </c>
+      <c r="E278" t="s">
+        <v>33</v>
+      </c>
+      <c r="F278" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B279" t="s">
+        <v>32</v>
+      </c>
+      <c r="C279" t="s">
+        <v>26</v>
+      </c>
+      <c r="D279" t="s">
+        <v>267</v>
+      </c>
+      <c r="E279" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B280" t="s">
+        <v>24</v>
+      </c>
+      <c r="D280" t="s">
+        <v>268</v>
+      </c>
+      <c r="E280" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A281" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A282" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B283" t="s">
+        <v>23</v>
+      </c>
+      <c r="D283" t="s">
+        <v>269</v>
+      </c>
+      <c r="E283" t="s">
+        <v>33</v>
+      </c>
+      <c r="F283" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B284" t="s">
+        <v>32</v>
+      </c>
+      <c r="C284" t="s">
+        <v>26</v>
+      </c>
+      <c r="D284" t="s">
+        <v>271</v>
+      </c>
+      <c r="E284" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B285" t="s">
+        <v>24</v>
+      </c>
+      <c r="D285" t="s">
+        <v>272</v>
+      </c>
+      <c r="E285" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A286" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="287" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A287" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B288" t="s">
+        <v>23</v>
+      </c>
+      <c r="D288" t="s">
+        <v>273</v>
+      </c>
+      <c r="E288" t="s">
+        <v>33</v>
+      </c>
+      <c r="F288" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B289" t="s">
+        <v>32</v>
+      </c>
+      <c r="C289" t="s">
+        <v>26</v>
+      </c>
+      <c r="D289" t="s">
+        <v>275</v>
+      </c>
+      <c r="E289" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B290" t="s">
+        <v>24</v>
+      </c>
+      <c r="D290" t="s">
+        <v>276</v>
+      </c>
+      <c r="E290" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A291" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A292" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B293" t="s">
+        <v>23</v>
+      </c>
+      <c r="D293" t="s">
+        <v>277</v>
+      </c>
+      <c r="E293" t="s">
+        <v>33</v>
+      </c>
+      <c r="F293" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B294" t="s">
+        <v>32</v>
+      </c>
+      <c r="C294" t="s">
+        <v>26</v>
+      </c>
+      <c r="D294" t="s">
+        <v>279</v>
+      </c>
+      <c r="E294" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B295" t="s">
+        <v>24</v>
+      </c>
+      <c r="D295" t="s">
+        <v>280</v>
+      </c>
+      <c r="E295" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A296" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A297" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B298" t="s">
+        <v>23</v>
+      </c>
+      <c r="D298" t="s">
+        <v>281</v>
+      </c>
+      <c r="E298" t="s">
+        <v>33</v>
+      </c>
+      <c r="F298" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B299" t="s">
+        <v>32</v>
+      </c>
+      <c r="C299" t="s">
+        <v>26</v>
+      </c>
+      <c r="D299" t="s">
+        <v>283</v>
+      </c>
+      <c r="E299" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B300" t="s">
+        <v>24</v>
+      </c>
+      <c r="D300" t="s">
+        <v>284</v>
+      </c>
+      <c r="E300" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A301" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A302" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B303" t="s">
+        <v>23</v>
+      </c>
+      <c r="D303" t="s">
+        <v>285</v>
+      </c>
+      <c r="E303" t="s">
+        <v>33</v>
+      </c>
+      <c r="F303" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B304" t="s">
+        <v>32</v>
+      </c>
+      <c r="C304" t="s">
+        <v>26</v>
+      </c>
+      <c r="D304" t="s">
+        <v>287</v>
+      </c>
+      <c r="E304" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B305" t="s">
+        <v>24</v>
+      </c>
+      <c r="D305" t="s">
+        <v>288</v>
+      </c>
+      <c r="E305" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A306" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A307" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="308" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B308" t="s">
+        <v>23</v>
+      </c>
+      <c r="D308" t="s">
+        <v>289</v>
+      </c>
+      <c r="E308" t="s">
+        <v>33</v>
+      </c>
+      <c r="F308" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B309" t="s">
+        <v>32</v>
+      </c>
+      <c r="C309" t="s">
+        <v>26</v>
+      </c>
+      <c r="D309" t="s">
+        <v>291</v>
+      </c>
+      <c r="E309" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="310" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B310" t="s">
+        <v>24</v>
+      </c>
+      <c r="D310" t="s">
+        <v>292</v>
+      </c>
+      <c r="E310" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="311" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A311" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="312" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A312" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="313" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B313" t="s">
+        <v>23</v>
+      </c>
+      <c r="D313" t="s">
+        <v>293</v>
+      </c>
+      <c r="E313" t="s">
+        <v>33</v>
+      </c>
+      <c r="F313" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="314" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B314" t="s">
+        <v>32</v>
+      </c>
+      <c r="C314" t="s">
+        <v>26</v>
+      </c>
+      <c r="D314" t="s">
+        <v>295</v>
+      </c>
+      <c r="E314" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="315" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B315" t="s">
+        <v>24</v>
+      </c>
+      <c r="D315" t="s">
+        <v>296</v>
+      </c>
+      <c r="E315" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="316" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A316" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="317" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A317" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="318" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B318" t="s">
+        <v>23</v>
+      </c>
+      <c r="D318" t="s">
+        <v>297</v>
+      </c>
+      <c r="E318" t="s">
+        <v>33</v>
+      </c>
+      <c r="F318" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="319" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B319" t="s">
+        <v>32</v>
+      </c>
+      <c r="C319" t="s">
+        <v>26</v>
+      </c>
+      <c r="D319" t="s">
+        <v>299</v>
+      </c>
+      <c r="E319" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="320" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B320" t="s">
+        <v>24</v>
+      </c>
+      <c r="D320" t="s">
+        <v>300</v>
+      </c>
+      <c r="E320" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="321" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A321" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="322" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A322" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="323" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B323" t="s">
+        <v>23</v>
+      </c>
+      <c r="D323" t="s">
+        <v>301</v>
+      </c>
+      <c r="E323" t="s">
+        <v>33</v>
+      </c>
+      <c r="F323" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="324" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B324" t="s">
+        <v>32</v>
+      </c>
+      <c r="C324" t="s">
+        <v>26</v>
+      </c>
+      <c r="D324" t="s">
+        <v>303</v>
+      </c>
+      <c r="E324" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="325" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B325" t="s">
+        <v>24</v>
+      </c>
+      <c r="D325" t="s">
+        <v>304</v>
+      </c>
+      <c r="E325" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="326" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A326" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="327" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A327" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="328" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B328" t="s">
+        <v>23</v>
+      </c>
+      <c r="D328" t="s">
+        <v>305</v>
+      </c>
+      <c r="E328" t="s">
+        <v>33</v>
+      </c>
+      <c r="F328" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="329" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B329" t="s">
+        <v>32</v>
+      </c>
+      <c r="C329" t="s">
+        <v>26</v>
+      </c>
+      <c r="D329" t="s">
+        <v>307</v>
+      </c>
+      <c r="E329" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="330" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B330" t="s">
+        <v>24</v>
+      </c>
+      <c r="D330" t="s">
+        <v>308</v>
+      </c>
+      <c r="E330" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="331" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A331" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="332" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A332" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="333" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B333" t="s">
+        <v>23</v>
+      </c>
+      <c r="D333" t="s">
+        <v>309</v>
+      </c>
+      <c r="E333" t="s">
+        <v>33</v>
+      </c>
+      <c r="F333" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="334" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B334" t="s">
+        <v>32</v>
+      </c>
+      <c r="C334" t="s">
+        <v>26</v>
+      </c>
+      <c r="D334" t="s">
+        <v>311</v>
+      </c>
+      <c r="E334" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="335" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B335" t="s">
+        <v>24</v>
+      </c>
+      <c r="D335" t="s">
+        <v>312</v>
+      </c>
+      <c r="E335" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="336" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A336" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="337" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A337" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="338" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B338" t="s">
+        <v>23</v>
+      </c>
+      <c r="D338" t="s">
+        <v>313</v>
+      </c>
+      <c r="E338" t="s">
+        <v>33</v>
+      </c>
+      <c r="F338" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="339" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B339" t="s">
+        <v>32</v>
+      </c>
+      <c r="C339" t="s">
+        <v>26</v>
+      </c>
+      <c r="D339" t="s">
+        <v>315</v>
+      </c>
+      <c r="E339" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="340" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B340" t="s">
+        <v>24</v>
+      </c>
+      <c r="D340" t="s">
+        <v>316</v>
+      </c>
+      <c r="E340" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="341" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A341" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="342" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A342" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="343" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B343" t="s">
+        <v>23</v>
+      </c>
+      <c r="D343" t="s">
+        <v>317</v>
+      </c>
+      <c r="E343" t="s">
+        <v>33</v>
+      </c>
+      <c r="F343" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="344" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B344" t="s">
+        <v>32</v>
+      </c>
+      <c r="C344" t="s">
+        <v>26</v>
+      </c>
+      <c r="D344" t="s">
+        <v>319</v>
+      </c>
+      <c r="E344" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="345" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B345" t="s">
+        <v>24</v>
+      </c>
+      <c r="D345" t="s">
+        <v>320</v>
+      </c>
+      <c r="E345" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="346" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A346" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="347" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A347" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="348" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B348" t="s">
+        <v>23</v>
+      </c>
+      <c r="D348" t="s">
+        <v>321</v>
+      </c>
+      <c r="E348" t="s">
+        <v>33</v>
+      </c>
+      <c r="F348" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="349" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B349" t="s">
+        <v>32</v>
+      </c>
+      <c r="C349" t="s">
+        <v>26</v>
+      </c>
+      <c r="D349" t="s">
+        <v>323</v>
+      </c>
+      <c r="E349" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="350" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B350" t="s">
+        <v>24</v>
+      </c>
+      <c r="D350" t="s">
+        <v>324</v>
+      </c>
+      <c r="E350" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="351" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A351" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="352" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A352" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="353" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B353" t="s">
+        <v>23</v>
+      </c>
+      <c r="D353" t="s">
+        <v>325</v>
+      </c>
+      <c r="E353" t="s">
+        <v>33</v>
+      </c>
+      <c r="F353" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="354" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B354" t="s">
+        <v>32</v>
+      </c>
+      <c r="C354" t="s">
+        <v>26</v>
+      </c>
+      <c r="D354" t="s">
+        <v>327</v>
+      </c>
+      <c r="E354" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="355" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B355" t="s">
+        <v>24</v>
+      </c>
+      <c r="D355" t="s">
+        <v>328</v>
+      </c>
+      <c r="E355" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="356" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A356" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="357" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A357" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="358" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B358" t="s">
+        <v>23</v>
+      </c>
+      <c r="D358" t="s">
+        <v>329</v>
+      </c>
+      <c r="E358" t="s">
+        <v>33</v>
+      </c>
+      <c r="F358" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="359" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B359" t="s">
+        <v>32</v>
+      </c>
+      <c r="C359" t="s">
+        <v>26</v>
+      </c>
+      <c r="D359" t="s">
+        <v>331</v>
+      </c>
+      <c r="E359" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="360" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B360" t="s">
+        <v>24</v>
+      </c>
+      <c r="D360" t="s">
+        <v>332</v>
+      </c>
+      <c r="E360" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="361" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A361" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="362" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A362" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="363" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B363" t="s">
+        <v>23</v>
+      </c>
+      <c r="D363" t="s">
+        <v>333</v>
+      </c>
+      <c r="E363" t="s">
+        <v>33</v>
+      </c>
+      <c r="F363" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="364" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B364" t="s">
+        <v>32</v>
+      </c>
+      <c r="C364" t="s">
+        <v>26</v>
+      </c>
+      <c r="D364" t="s">
+        <v>335</v>
+      </c>
+      <c r="E364" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="365" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B365" t="s">
+        <v>24</v>
+      </c>
+      <c r="D365" t="s">
+        <v>336</v>
+      </c>
+      <c r="E365" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="366" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A366" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="367" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A367" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="368" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B368" t="s">
+        <v>23</v>
+      </c>
+      <c r="D368" t="s">
+        <v>337</v>
+      </c>
+      <c r="E368" t="s">
+        <v>33</v>
+      </c>
+      <c r="F368" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="369" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B369" t="s">
+        <v>32</v>
+      </c>
+      <c r="C369" t="s">
+        <v>26</v>
+      </c>
+      <c r="D369" t="s">
+        <v>339</v>
+      </c>
+      <c r="E369" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="370" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B370" t="s">
+        <v>24</v>
+      </c>
+      <c r="D370" t="s">
+        <v>340</v>
+      </c>
+      <c r="E370" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="371" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A371" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="372" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A372" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="373" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B373" t="s">
+        <v>23</v>
+      </c>
+      <c r="D373" t="s">
+        <v>341</v>
+      </c>
+      <c r="E373" t="s">
+        <v>33</v>
+      </c>
+      <c r="F373" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="374" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B374" t="s">
+        <v>32</v>
+      </c>
+      <c r="C374" t="s">
+        <v>26</v>
+      </c>
+      <c r="D374" t="s">
+        <v>343</v>
+      </c>
+      <c r="E374" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="375" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B375" t="s">
+        <v>24</v>
+      </c>
+      <c r="D375" t="s">
+        <v>344</v>
+      </c>
+      <c r="E375" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="376" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A376" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="377" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A377" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="378" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B378" t="s">
+        <v>23</v>
+      </c>
+      <c r="D378" t="s">
+        <v>345</v>
+      </c>
+      <c r="E378" t="s">
+        <v>33</v>
+      </c>
+      <c r="F378" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="379" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B379" t="s">
+        <v>32</v>
+      </c>
+      <c r="C379" t="s">
+        <v>26</v>
+      </c>
+      <c r="D379" t="s">
+        <v>347</v>
+      </c>
+      <c r="E379" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="380" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B380" t="s">
+        <v>24</v>
+      </c>
+      <c r="D380" t="s">
+        <v>348</v>
+      </c>
+      <c r="E380" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="381" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A381" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2649,7 +5334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AFEF6AD-8C74-41B4-8E24-8AA1ECBF8E0A}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>

</xml_diff>